<commit_message>
Projektmanagement versendet an Herr Jensen
</commit_message>
<xml_diff>
--- a/Projektmanagement/Risikoanalyse.xlsx
+++ b/Projektmanagement/Risikoanalyse.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Risikoanalyse" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="64">
   <si>
     <t>&lt;Ihr Logo&gt;</t>
   </si>
@@ -187,12 +187,6 @@
     <t>Beispiel 1</t>
   </si>
   <si>
-    <t>Beispiel 2</t>
-  </si>
-  <si>
-    <t>Beispiel 3</t>
-  </si>
-  <si>
     <t>Beispiel 4</t>
   </si>
   <si>
@@ -209,9 +203,6 @@
  - Änderungsgrund 2…</t>
   </si>
   <si>
-    <t>Risikoanalyse &lt;3D Laserscanner für mobile Roboter&gt;</t>
-  </si>
-  <si>
     <t>nicht eingetroffen</t>
   </si>
   <si>
@@ -237,26 +228,44 @@
     <t>Lieferengpässe / Komponenten nicht verfügbar</t>
   </si>
   <si>
-    <t>Liefertermin und Stückzahl beachten</t>
-  </si>
-  <si>
-    <t>Regelmässiger Abgleich mit Kunde</t>
-  </si>
-  <si>
     <t>gleichwertige Alternativen suchen und evaluieren, Projektplanung ändern</t>
   </si>
   <si>
     <t>Materialverlust / Diebstahl</t>
+  </si>
+  <si>
+    <t>Liefertermine und Stückzahl frühzeitig kontrollieren</t>
+  </si>
+  <si>
+    <t>Dokumentation</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>Hardware</t>
+  </si>
+  <si>
+    <t>Material geschutzt verräumen,</t>
+  </si>
+  <si>
+    <t>Alternative</t>
+  </si>
+  <si>
+    <t>Regelmässiger Abgleich mit Dozent</t>
+  </si>
+  <si>
+    <t>Risikoanalyse &lt;3D Laserscanner für mobiler Roboter&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="180" formatCode="#,##0;\(#,##0\)"/>
+    <numFmt numFmtId="164" formatCode="#,##0;\(#,##0\)"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -333,12 +342,6 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <color indexed="10"/>
       <name val="Tahoma"/>
@@ -362,6 +365,17 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="10"/>
       <color indexed="9"/>
@@ -369,19 +383,14 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b/>
+      <sz val="8"/>
+      <color indexed="9"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color indexed="9"/>
+      <sz val="11"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -394,8 +403,17 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <sz val="9"/>
       <color indexed="23"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -895,12 +913,12 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -926,149 +944,27 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="180" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="180" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="180" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="180" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="18" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="18" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="21" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="18" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="18" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="18" fillId="5" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="18" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="18" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="18" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="18" fillId="5" borderId="15" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="18" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="6" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="6" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="6" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="180" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1105,33 +1001,158 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="19" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="5" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="5" borderId="15" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="6" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="6" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="6" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -1537,7 +1558,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -1613,73 +1634,73 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
-      <c r="B7" s="74" t="s">
+      <c r="B7" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="76"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="32"/>
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
-      <c r="B8" s="77"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="78"/>
-      <c r="F8" s="79"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="35"/>
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
-      <c r="B9" s="77" t="s">
+      <c r="B9" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="78"/>
-      <c r="D9" s="78"/>
-      <c r="E9" s="78"/>
-      <c r="F9" s="79"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="35"/>
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
-      <c r="B10" s="77"/>
-      <c r="C10" s="78"/>
-      <c r="D10" s="78"/>
-      <c r="E10" s="78"/>
-      <c r="F10" s="79"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="35"/>
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
-      <c r="B11" s="77" t="s">
+      <c r="B11" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="78"/>
-      <c r="D11" s="78"/>
-      <c r="E11" s="78"/>
-      <c r="F11" s="79"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="35"/>
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
-      <c r="B12" s="83" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="84"/>
-      <c r="D12" s="84"/>
-      <c r="E12" s="84"/>
-      <c r="F12" s="85"/>
+      <c r="B12" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="41"/>
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
-      <c r="B13" s="80"/>
-      <c r="C13" s="81"/>
-      <c r="D13" s="81"/>
-      <c r="E13" s="81"/>
-      <c r="F13" s="82"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="38"/>
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -2026,8 +2047,8 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C21" location="Historie!A1" display="zur Versionshistorie"/>
-    <hyperlink ref="C22" location="Details!A1" display="zu den Details"/>
+    <hyperlink ref="C21" location="Historie!A1" display="zur Versionshistorie" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C22" location="Details!A1" display="zu den Details" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2036,7 +2057,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -2067,7 +2088,7 @@
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7"/>
       <c r="B2" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -2104,10 +2125,10 @@
       <c r="D5" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="90" t="s">
+      <c r="E5" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="91"/>
+      <c r="F5" s="47"/>
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -2117,10 +2138,10 @@
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
-      <c r="E6" s="86" t="s">
+      <c r="E6" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="87"/>
+      <c r="F6" s="43"/>
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
@@ -2130,10 +2151,10 @@
       </c>
       <c r="C7" s="23"/>
       <c r="D7" s="23"/>
-      <c r="E7" s="92" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" s="87"/>
+      <c r="E7" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="43"/>
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -2141,8 +2162,8 @@
       <c r="B8" s="24"/>
       <c r="C8" s="23"/>
       <c r="D8" s="23"/>
-      <c r="E8" s="86"/>
-      <c r="F8" s="87"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="43"/>
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2150,8 +2171,8 @@
       <c r="B9" s="24"/>
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="87"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="43"/>
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -2159,8 +2180,8 @@
       <c r="B10" s="24"/>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="87"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="43"/>
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -2168,8 +2189,8 @@
       <c r="B11" s="25"/>
       <c r="C11" s="26"/>
       <c r="D11" s="26"/>
-      <c r="E11" s="88"/>
-      <c r="F11" s="89"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="45"/>
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -2487,841 +2508,847 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="1.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" style="31" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" style="30" customWidth="1"/>
-    <col min="4" max="5" width="5.140625" style="30" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="30" customWidth="1"/>
-    <col min="7" max="7" width="36.5703125" style="30" customWidth="1"/>
-    <col min="8" max="8" width="33.85546875" style="31" customWidth="1"/>
-    <col min="9" max="9" width="38.28515625" style="31" customWidth="1"/>
-    <col min="10" max="10" width="24.5703125" style="31" customWidth="1"/>
-    <col min="11" max="11" width="21.85546875" style="31" customWidth="1"/>
-    <col min="12" max="14" width="12.7109375" style="31" customWidth="1"/>
-    <col min="15" max="15" width="15.85546875" style="31" customWidth="1"/>
-    <col min="16" max="16384" width="12.7109375" style="31"/>
+    <col min="1" max="1" width="1.28515625" style="96" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="52" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" style="51" customWidth="1"/>
+    <col min="4" max="5" width="5.140625" style="51" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="51" customWidth="1"/>
+    <col min="7" max="7" width="36.5703125" style="51" customWidth="1"/>
+    <col min="8" max="8" width="33.85546875" style="52" customWidth="1"/>
+    <col min="9" max="9" width="38.28515625" style="52" customWidth="1"/>
+    <col min="10" max="10" width="24.5703125" style="52" customWidth="1"/>
+    <col min="11" max="11" width="21.85546875" style="52" customWidth="1"/>
+    <col min="12" max="14" width="12.7109375" style="52" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" style="52" customWidth="1"/>
+    <col min="16" max="16384" width="12.7109375" style="52"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5"/>
-      <c r="B1" s="54" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" s="32" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="56" t="s">
+      <c r="A1" s="49"/>
+      <c r="B1" s="50" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="57" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="53"/>
+      <c r="B2" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="58" t="s">
+      <c r="D2" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="58" t="s">
+      <c r="E2" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="57" t="s">
+      <c r="F2" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="57" t="s">
+      <c r="H2" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="57" t="s">
+      <c r="I2" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="57" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" s="32" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="5"/>
-      <c r="B3" s="59" t="s">
+      <c r="J2" s="55" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="57" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="49"/>
+      <c r="B3" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="62"/>
-      <c r="M3" s="71" t="s">
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="61"/>
+      <c r="M3" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="N3" s="71" t="s">
+      <c r="N3" s="62" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="38" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="5"/>
-      <c r="B4" s="33" t="s">
+    <row r="4" spans="1:14" s="70" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A4" s="49"/>
+      <c r="B4" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="67">
+      <c r="C4" s="64">
         <v>1</v>
       </c>
-      <c r="D4" s="34">
+      <c r="D4" s="65">
         <v>0</v>
       </c>
-      <c r="E4" s="34">
+      <c r="E4" s="65">
         <v>1</v>
       </c>
-      <c r="F4" s="35">
+      <c r="F4" s="66">
         <f t="shared" ref="F4:F14" si="0">D4*E4</f>
         <v>0</v>
       </c>
-      <c r="G4" s="93" t="s">
+      <c r="G4" s="67" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="H4" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="I4" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="J4" s="94" t="s">
-        <v>59</v>
-      </c>
-      <c r="M4" s="72">
+      <c r="I4" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="M4" s="71">
         <v>0</v>
       </c>
-      <c r="N4" s="72" t="s">
+      <c r="N4" s="71" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
-      <c r="B5" s="33" t="s">
+    <row r="5" spans="1:14" s="70" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="49"/>
+      <c r="B5" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="67">
+      <c r="C5" s="64">
         <v>2</v>
       </c>
-      <c r="D5" s="34">
+      <c r="D5" s="65">
         <v>1</v>
       </c>
-      <c r="E5" s="34">
-        <v>2</v>
-      </c>
-      <c r="F5" s="35">
+      <c r="E5" s="65">
+        <v>4</v>
+      </c>
+      <c r="F5" s="66">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G5" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="68" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="J5" s="37"/>
-      <c r="M5" s="72">
+      <c r="I5" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5" s="72" t="s">
+        <v>61</v>
+      </c>
+      <c r="M5" s="71">
         <v>1</v>
       </c>
-      <c r="N5" s="72" t="s">
+      <c r="N5" s="71" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-      <c r="B6" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="67">
+    <row r="6" spans="1:14" s="70" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="49"/>
+      <c r="B6" s="63" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="64">
         <v>3</v>
       </c>
-      <c r="D6" s="34">
+      <c r="D6" s="65">
         <v>3</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="65">
         <v>3</v>
       </c>
-      <c r="F6" s="35">
+      <c r="F6" s="66">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="J6" s="37"/>
-      <c r="M6" s="72">
+      <c r="G6" s="68"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="72"/>
+      <c r="M6" s="71">
         <v>2</v>
       </c>
-      <c r="N6" s="72" t="s">
+      <c r="N6" s="71" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="33" t="s">
+    <row r="7" spans="1:14" s="70" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="49"/>
+      <c r="B7" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="67">
+      <c r="C7" s="64">
         <v>4</v>
       </c>
-      <c r="D7" s="34">
+      <c r="D7" s="65">
         <v>0</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="65">
         <v>0</v>
       </c>
-      <c r="F7" s="35">
+      <c r="F7" s="66">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="J7" s="37"/>
-      <c r="M7" s="72">
+      <c r="G7" s="68"/>
+      <c r="H7" s="68"/>
+      <c r="I7" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" s="72"/>
+      <c r="M7" s="71">
         <v>3</v>
       </c>
-      <c r="N7" s="72" t="s">
+      <c r="N7" s="71" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="38" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="33" t="s">
+    <row r="8" spans="1:14" s="70" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="49"/>
+      <c r="B8" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="67">
+      <c r="C8" s="64">
         <v>5</v>
       </c>
-      <c r="D8" s="34">
+      <c r="D8" s="65">
         <v>0</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="65">
         <v>0</v>
       </c>
-      <c r="F8" s="35">
+      <c r="F8" s="66">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="J8" s="37"/>
-      <c r="M8" s="72"/>
-      <c r="N8" s="72" t="s">
+      <c r="G8" s="68"/>
+      <c r="H8" s="68"/>
+      <c r="I8" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="J8" s="72"/>
+      <c r="M8" s="71"/>
+      <c r="N8" s="71" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="67">
+    <row r="9" spans="1:14" s="70" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="49"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="64">
         <v>6</v>
       </c>
-      <c r="D9" s="34">
+      <c r="D9" s="65">
         <v>0</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="65">
         <v>0</v>
       </c>
-      <c r="F9" s="35">
+      <c r="F9" s="66">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="J9" s="37"/>
-      <c r="M9" s="72"/>
-      <c r="N9" s="72" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="67">
+      <c r="G9" s="68"/>
+      <c r="H9" s="68"/>
+      <c r="I9" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" s="72"/>
+      <c r="M9" s="71"/>
+      <c r="N9" s="71" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" s="70" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="49"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="64">
         <v>7</v>
       </c>
-      <c r="D10" s="34">
+      <c r="D10" s="65">
         <v>0</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E10" s="65">
         <v>0</v>
       </c>
-      <c r="F10" s="35">
+      <c r="F10" s="66">
         <f>D10*E10</f>
         <v>0</v>
       </c>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="J10" s="37"/>
-      <c r="M10" s="72"/>
-      <c r="N10" s="72" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="67">
+      <c r="G10" s="68"/>
+      <c r="H10" s="68"/>
+      <c r="I10" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" s="72"/>
+      <c r="M10" s="71"/>
+      <c r="N10" s="71" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="70" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="49"/>
+      <c r="B11" s="63"/>
+      <c r="C11" s="64">
         <v>8</v>
       </c>
-      <c r="D11" s="34">
+      <c r="D11" s="65">
         <v>0</v>
       </c>
-      <c r="E11" s="34">
+      <c r="E11" s="65">
         <v>0</v>
       </c>
-      <c r="F11" s="35">
+      <c r="F11" s="66">
         <f>D11*E11</f>
         <v>0</v>
       </c>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="J11" s="37"/>
-      <c r="M11" s="72"/>
-      <c r="N11" s="72" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="67">
+      <c r="G11" s="68"/>
+      <c r="H11" s="68"/>
+      <c r="I11" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="J11" s="72"/>
+      <c r="M11" s="71"/>
+      <c r="N11" s="71" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="70" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="49"/>
+      <c r="B12" s="63"/>
+      <c r="C12" s="64">
         <v>9</v>
       </c>
-      <c r="D12" s="34">
+      <c r="D12" s="65">
         <v>0</v>
       </c>
-      <c r="E12" s="34">
+      <c r="E12" s="65">
         <v>0</v>
       </c>
-      <c r="F12" s="35">
+      <c r="F12" s="66">
         <f>D12*E12</f>
         <v>0</v>
       </c>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="J12" s="37"/>
-      <c r="M12" s="72"/>
-      <c r="N12" s="72" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="67"/>
-      <c r="D13" s="34">
+      <c r="G12" s="68"/>
+      <c r="H12" s="68"/>
+      <c r="I12" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="J12" s="72"/>
+      <c r="M12" s="71"/>
+      <c r="N12" s="71" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="70" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="49"/>
+      <c r="B13" s="63"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="65">
         <v>0</v>
       </c>
-      <c r="E13" s="34">
+      <c r="E13" s="65">
         <v>0</v>
       </c>
-      <c r="F13" s="35">
+      <c r="F13" s="66">
         <f>D13*E13</f>
         <v>0</v>
       </c>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="J13" s="37"/>
-      <c r="M13" s="72"/>
-      <c r="N13" s="72"/>
-    </row>
-    <row r="14" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="5"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="67">
+      <c r="G13" s="68"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="J13" s="72"/>
+      <c r="M13" s="71"/>
+      <c r="N13" s="71"/>
+    </row>
+    <row r="14" spans="1:14" s="70" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="49"/>
+      <c r="B14" s="63"/>
+      <c r="C14" s="64">
         <v>10</v>
       </c>
-      <c r="D14" s="34">
+      <c r="D14" s="65">
         <v>0</v>
       </c>
-      <c r="E14" s="34">
+      <c r="E14" s="65">
         <v>0</v>
       </c>
-      <c r="F14" s="35">
+      <c r="F14" s="66">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="J14" s="37"/>
-      <c r="M14" s="72"/>
-      <c r="N14" s="72" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" s="32" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="63" t="s">
+      <c r="G14" s="68"/>
+      <c r="H14" s="68"/>
+      <c r="I14" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="J14" s="72"/>
+      <c r="M14" s="71"/>
+      <c r="N14" s="71" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="57" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="49"/>
+      <c r="B15" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="64"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="65"/>
-      <c r="G15" s="64"/>
-      <c r="H15" s="64"/>
-      <c r="I15" s="64"/>
-      <c r="J15" s="66"/>
-      <c r="M15" s="73"/>
-      <c r="N15" s="72" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" s="38" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="5"/>
-      <c r="B16" s="39" t="s">
+      <c r="C15" s="74"/>
+      <c r="D15" s="74"/>
+      <c r="E15" s="74"/>
+      <c r="F15" s="75"/>
+      <c r="G15" s="74"/>
+      <c r="H15" s="74"/>
+      <c r="I15" s="74"/>
+      <c r="J15" s="76"/>
+      <c r="M15" s="77"/>
+      <c r="N15" s="71" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" s="70" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="49"/>
+      <c r="B16" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="68">
+      <c r="C16" s="79">
         <v>11</v>
       </c>
-      <c r="D16" s="40">
+      <c r="D16" s="80">
         <v>3</v>
       </c>
-      <c r="E16" s="40">
+      <c r="E16" s="80">
         <v>1</v>
       </c>
-      <c r="F16" s="35">
+      <c r="F16" s="66">
         <f>D16*E16</f>
         <v>3</v>
       </c>
-      <c r="G16" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="H16" s="41" t="s">
-        <v>58</v>
-      </c>
-      <c r="I16" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="J16" s="42"/>
-    </row>
-    <row r="17" spans="1:10" s="38" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="5"/>
-      <c r="B17" s="39" t="s">
+      <c r="G16" s="81" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16" s="81" t="s">
+        <v>62</v>
+      </c>
+      <c r="I16" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="J16" s="82"/>
+    </row>
+    <row r="17" spans="1:10" s="70" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="49"/>
+      <c r="B17" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="68">
+      <c r="C17" s="79">
         <v>12</v>
       </c>
-      <c r="D17" s="40">
+      <c r="D17" s="80">
         <v>3</v>
       </c>
-      <c r="E17" s="40">
+      <c r="E17" s="80">
         <v>2</v>
       </c>
-      <c r="F17" s="35">
+      <c r="F17" s="66">
         <f>D17*E17</f>
         <v>6</v>
       </c>
-      <c r="G17" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="H17" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="I17" s="36" t="s">
+      <c r="G17" s="83" t="s">
+        <v>48</v>
+      </c>
+      <c r="H17" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="J17" s="42"/>
-    </row>
-    <row r="18" spans="1:10" s="38" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5"/>
-      <c r="B18" s="33" t="s">
+      <c r="I17" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="J17" s="82"/>
+    </row>
+    <row r="18" spans="1:10" s="70" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="49"/>
+      <c r="B18" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="69">
+      <c r="C18" s="84">
         <v>13</v>
       </c>
-      <c r="D18" s="34">
+      <c r="D18" s="65">
         <v>2</v>
       </c>
-      <c r="E18" s="34">
+      <c r="E18" s="65">
         <v>2</v>
       </c>
-      <c r="F18" s="35">
+      <c r="F18" s="66">
         <f>D18*E18</f>
         <v>4</v>
       </c>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="J18" s="37"/>
-    </row>
-    <row r="19" spans="1:10" s="38" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="5"/>
-      <c r="B19" s="33"/>
-      <c r="C19" s="69">
+      <c r="G18" s="68"/>
+      <c r="H18" s="68"/>
+      <c r="I18" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="J18" s="72"/>
+    </row>
+    <row r="19" spans="1:10" s="70" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="49"/>
+      <c r="B19" s="63"/>
+      <c r="C19" s="84">
         <v>14</v>
       </c>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="J19" s="37"/>
-    </row>
-    <row r="20" spans="1:10" s="38" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="5"/>
-      <c r="B20" s="33"/>
-      <c r="C20" s="69">
+      <c r="D19" s="65"/>
+      <c r="E19" s="65"/>
+      <c r="F19" s="66"/>
+      <c r="G19" s="68"/>
+      <c r="H19" s="68"/>
+      <c r="I19" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="J19" s="72"/>
+    </row>
+    <row r="20" spans="1:10" s="70" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="49"/>
+      <c r="B20" s="63"/>
+      <c r="C20" s="84">
         <v>15</v>
       </c>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="J20" s="37"/>
-    </row>
-    <row r="21" spans="1:10" s="38" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="5"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="69">
+      <c r="D20" s="65"/>
+      <c r="E20" s="65"/>
+      <c r="F20" s="66"/>
+      <c r="G20" s="68"/>
+      <c r="H20" s="68"/>
+      <c r="I20" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="J20" s="72"/>
+    </row>
+    <row r="21" spans="1:10" s="70" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="49"/>
+      <c r="B21" s="63"/>
+      <c r="C21" s="84">
         <v>16</v>
       </c>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="J21" s="37"/>
-    </row>
-    <row r="22" spans="1:10" s="38" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="69">
+      <c r="D21" s="65"/>
+      <c r="E21" s="65"/>
+      <c r="F21" s="66"/>
+      <c r="G21" s="68"/>
+      <c r="H21" s="68"/>
+      <c r="I21" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="J21" s="72"/>
+    </row>
+    <row r="22" spans="1:10" s="70" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="49"/>
+      <c r="B22" s="63"/>
+      <c r="C22" s="84">
         <v>17</v>
       </c>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="J22" s="37"/>
-    </row>
-    <row r="23" spans="1:10" s="38" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="5"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="69">
+      <c r="D22" s="65"/>
+      <c r="E22" s="65"/>
+      <c r="F22" s="66"/>
+      <c r="G22" s="68"/>
+      <c r="H22" s="68"/>
+      <c r="I22" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="J22" s="72"/>
+    </row>
+    <row r="23" spans="1:10" s="70" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="49"/>
+      <c r="B23" s="63"/>
+      <c r="C23" s="84">
         <v>18</v>
       </c>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="J23" s="37"/>
-    </row>
-    <row r="24" spans="1:10" s="38" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="5"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="69">
+      <c r="D23" s="65"/>
+      <c r="E23" s="65"/>
+      <c r="F23" s="66"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="J23" s="72"/>
+    </row>
+    <row r="24" spans="1:10" s="70" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="49"/>
+      <c r="B24" s="63"/>
+      <c r="C24" s="84">
         <v>19</v>
       </c>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="J24" s="37"/>
-    </row>
-    <row r="25" spans="1:10" s="38" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="5"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="69">
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="66"/>
+      <c r="G24" s="68"/>
+      <c r="H24" s="68"/>
+      <c r="I24" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="J24" s="72"/>
+    </row>
+    <row r="25" spans="1:10" s="70" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="49"/>
+      <c r="B25" s="63"/>
+      <c r="C25" s="84">
         <v>20</v>
       </c>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="J25" s="37"/>
-    </row>
-    <row r="26" spans="1:10" s="38" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="5"/>
-      <c r="B26" s="33"/>
-      <c r="C26" s="69" t="s">
+      <c r="D25" s="65"/>
+      <c r="E25" s="65"/>
+      <c r="F25" s="66"/>
+      <c r="G25" s="68"/>
+      <c r="H25" s="68"/>
+      <c r="I25" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="J25" s="72"/>
+    </row>
+    <row r="26" spans="1:10" s="70" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="49"/>
+      <c r="B26" s="63"/>
+      <c r="C26" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="J26" s="37"/>
-    </row>
-    <row r="27" spans="1:10" s="38" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="44"/>
-      <c r="C27" s="70" t="s">
+      <c r="D26" s="65"/>
+      <c r="E26" s="65"/>
+      <c r="F26" s="66"/>
+      <c r="G26" s="68"/>
+      <c r="H26" s="68"/>
+      <c r="I26" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="J26" s="72"/>
+    </row>
+    <row r="27" spans="1:10" s="70" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="49"/>
+      <c r="B27" s="85"/>
+      <c r="C27" s="86" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="45"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="55"/>
-      <c r="G27" s="46"/>
-      <c r="H27" s="46"/>
-      <c r="I27" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="J27" s="47"/>
-    </row>
-    <row r="28" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="5"/>
-      <c r="B28" s="48"/>
-      <c r="C28" s="49"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="49"/>
-      <c r="H28" s="48"/>
-    </row>
-    <row r="29" spans="1:10" s="50" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="63" t="s">
-        <v>55</v>
-      </c>
-      <c r="C29" s="64"/>
-      <c r="D29" s="64"/>
-      <c r="E29" s="64"/>
-      <c r="F29" s="65"/>
-      <c r="G29" s="64"/>
-      <c r="H29" s="64"/>
-      <c r="I29" s="64"/>
-      <c r="J29" s="66"/>
-    </row>
-    <row r="30" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="5"/>
-      <c r="B30" s="39" t="s">
+      <c r="D27" s="87"/>
+      <c r="E27" s="87"/>
+      <c r="F27" s="88"/>
+      <c r="G27" s="89"/>
+      <c r="H27" s="89"/>
+      <c r="I27" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="J27" s="90"/>
+    </row>
+    <row r="28" spans="1:10" s="93" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="49"/>
+      <c r="B28" s="91"/>
+      <c r="C28" s="92"/>
+      <c r="D28" s="92"/>
+      <c r="E28" s="92"/>
+      <c r="F28" s="92"/>
+      <c r="G28" s="92"/>
+      <c r="H28" s="91"/>
+    </row>
+    <row r="29" spans="1:10" s="93" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="49"/>
+      <c r="B29" s="73" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="74"/>
+      <c r="D29" s="74"/>
+      <c r="E29" s="74"/>
+      <c r="F29" s="75"/>
+      <c r="G29" s="74"/>
+      <c r="H29" s="74"/>
+      <c r="I29" s="74"/>
+      <c r="J29" s="76"/>
+    </row>
+    <row r="30" spans="1:10" s="93" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="49"/>
+      <c r="B30" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="68">
+      <c r="C30" s="79">
         <v>21</v>
       </c>
-      <c r="D30" s="40">
+      <c r="D30" s="80">
         <v>3</v>
       </c>
-      <c r="E30" s="40">
+      <c r="E30" s="80">
         <v>1</v>
       </c>
-      <c r="F30" s="35">
+      <c r="F30" s="66">
         <f>D30*E30</f>
         <v>3</v>
       </c>
-      <c r="G30" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="H30" s="41"/>
-      <c r="I30" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="J30" s="42"/>
-    </row>
-    <row r="31" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="5"/>
-      <c r="B31" s="39" t="s">
+      <c r="G30" s="81" t="s">
+        <v>50</v>
+      </c>
+      <c r="H30" s="81" t="s">
+        <v>62</v>
+      </c>
+      <c r="I30" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="J30" s="82"/>
+    </row>
+    <row r="31" spans="1:10" s="93" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="49"/>
+      <c r="B31" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="C31" s="68">
+      <c r="C31" s="79">
         <v>22</v>
       </c>
-      <c r="D31" s="40">
+      <c r="D31" s="80">
         <v>3</v>
       </c>
-      <c r="E31" s="40">
+      <c r="E31" s="80">
         <v>2</v>
       </c>
-      <c r="F31" s="35">
+      <c r="F31" s="66">
         <f>D31*E31</f>
         <v>6</v>
       </c>
-      <c r="G31" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="H31" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="I31" s="36" t="s">
+      <c r="G31" s="83" t="s">
+        <v>48</v>
+      </c>
+      <c r="H31" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="J31" s="42"/>
-    </row>
-    <row r="32" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="5"/>
-      <c r="B32" s="33" t="s">
+      <c r="I31" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="J31" s="82"/>
+    </row>
+    <row r="32" spans="1:10" s="93" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="49"/>
+      <c r="B32" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="69">
+      <c r="C32" s="84">
         <v>23</v>
       </c>
-      <c r="D32" s="34">
+      <c r="D32" s="65">
         <v>2</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="65">
         <v>2</v>
       </c>
-      <c r="F32" s="35">
+      <c r="F32" s="66">
         <f>D32*E32</f>
         <v>4</v>
       </c>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="J32" s="37"/>
-    </row>
-    <row r="33" spans="1:7" s="50" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="5"/>
-      <c r="C33" s="51"/>
-      <c r="D33" s="51"/>
-      <c r="E33" s="51"/>
-      <c r="F33" s="51"/>
-      <c r="G33" s="51"/>
-    </row>
-    <row r="34" spans="1:7" s="50" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="5"/>
-      <c r="C34" s="51"/>
-      <c r="D34" s="51"/>
-      <c r="E34" s="51"/>
-      <c r="F34" s="51"/>
-      <c r="G34" s="51"/>
-    </row>
-    <row r="35" spans="1:7" s="50" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="5"/>
-      <c r="C35" s="51"/>
-      <c r="D35" s="51"/>
-      <c r="E35" s="51"/>
-      <c r="F35" s="51"/>
-      <c r="G35" s="51"/>
-    </row>
-    <row r="36" spans="1:7" s="50" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="5"/>
-      <c r="C36" s="51"/>
-      <c r="D36" s="51"/>
-      <c r="E36" s="51"/>
-      <c r="F36" s="51"/>
-      <c r="G36" s="51"/>
-    </row>
-    <row r="37" spans="1:7" s="50" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A37" s="5"/>
-      <c r="B37" s="52"/>
-      <c r="C37" s="51"/>
-      <c r="D37" s="51"/>
-      <c r="E37" s="51"/>
-      <c r="F37" s="51"/>
-      <c r="G37" s="51"/>
-    </row>
-    <row r="38" spans="1:7" s="50" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="5"/>
-      <c r="C38" s="51"/>
-      <c r="D38" s="51"/>
-      <c r="E38" s="51"/>
-      <c r="F38" s="51"/>
-      <c r="G38" s="51"/>
-    </row>
-    <row r="39" spans="1:7" s="50" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="5"/>
-    </row>
-    <row r="40" spans="1:7" s="50" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="5"/>
-      <c r="C40" s="51"/>
-      <c r="D40" s="51"/>
-      <c r="E40" s="51"/>
-      <c r="F40" s="51"/>
-      <c r="G40" s="51"/>
-    </row>
-    <row r="41" spans="1:7" s="50" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="5"/>
-      <c r="C41" s="51"/>
-      <c r="D41" s="51"/>
-      <c r="E41" s="51"/>
-      <c r="F41" s="51"/>
-      <c r="G41" s="51"/>
-    </row>
-    <row r="42" spans="1:7" s="50" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="5"/>
-      <c r="B42" s="31"/>
-      <c r="C42" s="51"/>
-      <c r="D42" s="51"/>
-      <c r="E42" s="51"/>
-      <c r="F42" s="51"/>
-      <c r="G42" s="51"/>
+      <c r="G32" s="68"/>
+      <c r="H32" s="68"/>
+      <c r="I32" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="J32" s="72"/>
+    </row>
+    <row r="33" spans="1:7" s="93" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="49"/>
+      <c r="C33" s="94"/>
+      <c r="D33" s="94"/>
+      <c r="E33" s="94"/>
+      <c r="F33" s="94"/>
+      <c r="G33" s="94"/>
+    </row>
+    <row r="34" spans="1:7" s="93" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="49"/>
+      <c r="C34" s="94"/>
+      <c r="D34" s="94"/>
+      <c r="E34" s="94"/>
+      <c r="F34" s="94"/>
+      <c r="G34" s="94"/>
+    </row>
+    <row r="35" spans="1:7" s="93" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="49"/>
+      <c r="C35" s="94"/>
+      <c r="D35" s="94"/>
+      <c r="E35" s="94"/>
+      <c r="F35" s="94"/>
+      <c r="G35" s="94"/>
+    </row>
+    <row r="36" spans="1:7" s="93" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="49"/>
+      <c r="C36" s="94"/>
+      <c r="D36" s="94"/>
+      <c r="E36" s="94"/>
+      <c r="F36" s="94"/>
+      <c r="G36" s="94"/>
+    </row>
+    <row r="37" spans="1:7" s="93" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A37" s="49"/>
+      <c r="B37" s="95"/>
+      <c r="C37" s="94"/>
+      <c r="D37" s="94"/>
+      <c r="E37" s="94"/>
+      <c r="F37" s="94"/>
+      <c r="G37" s="94"/>
+    </row>
+    <row r="38" spans="1:7" s="93" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="49"/>
+      <c r="C38" s="94"/>
+      <c r="D38" s="94"/>
+      <c r="E38" s="94"/>
+      <c r="F38" s="94"/>
+      <c r="G38" s="94"/>
+    </row>
+    <row r="39" spans="1:7" s="93" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="49"/>
+    </row>
+    <row r="40" spans="1:7" s="93" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="49"/>
+      <c r="C40" s="94"/>
+      <c r="D40" s="94"/>
+      <c r="E40" s="94"/>
+      <c r="F40" s="94"/>
+      <c r="G40" s="94"/>
+    </row>
+    <row r="41" spans="1:7" s="93" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="49"/>
+      <c r="C41" s="94"/>
+      <c r="D41" s="94"/>
+      <c r="E41" s="94"/>
+      <c r="F41" s="94"/>
+      <c r="G41" s="94"/>
+    </row>
+    <row r="42" spans="1:7" s="93" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="49"/>
+      <c r="B42" s="52"/>
+      <c r="C42" s="94"/>
+      <c r="D42" s="94"/>
+      <c r="E42" s="94"/>
+      <c r="F42" s="94"/>
+      <c r="G42" s="94"/>
     </row>
     <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="B45" s="53"/>
+      <c r="B45" s="97"/>
     </row>
     <row r="50" spans="2:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="B50" s="53"/>
+      <c r="B50" s="97"/>
     </row>
     <row r="53" spans="2:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="B53" s="53"/>
+      <c r="B53" s="97"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -3363,10 +3390,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations xWindow="85" yWindow="491" count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="0=kein bis 3=sehr hoch" sqref="D16:E27 D4:E14 D30:E32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="0=kein bis 3=sehr hoch" sqref="D16:E27 D4:E14 D30:E32" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>$M$4:$M$8</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Typen / Klassen definieren" prompt="Geben Sie neue Risikotypen oder Klassen in der Spalte O ein" sqref="B16:B27 B30:B32 B4:B14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Typen / Klassen definieren" prompt="Geben Sie neue Risikotypen oder Klassen in der Spalte O ein" sqref="B16:B27 B30:B32 B4:B14" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>$N$4:$N$16</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>